<commit_message>
Implement possibility to export images.
</commit_message>
<xml_diff>
--- a/Features To Implement.xlsx
+++ b/Features To Implement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\InnovatorDataModelEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4452D159-8314-4208-BAFE-C5692E6ADE47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1BDC33-7AEB-4E9B-9001-ACF48F6552C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BCFEDF59-FA17-40DF-9E71-4D244AE6C829}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
   <si>
     <t>Import/Export from/to AML</t>
   </si>
@@ -69,12 +69,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -89,8 +95,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,7 +415,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,7 +445,7 @@
         <f t="shared" ref="B4:B10" si="0">B3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement possibility to print.
</commit_message>
<xml_diff>
--- a/Features To Implement.xlsx
+++ b/Features To Implement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\InnovatorDataModelEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1BDC33-7AEB-4E9B-9001-ACF48F6552C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38794F1-2718-4222-89BE-CCFBD8E817FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BCFEDF59-FA17-40DF-9E71-4D244AE6C829}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Import/Export from/to AML</t>
   </si>
@@ -454,7 +454,7 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement possibility to Copy+Paste items.
</commit_message>
<xml_diff>
--- a/Features To Implement.xlsx
+++ b/Features To Implement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\InnovatorDataModelEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38794F1-2718-4222-89BE-CCFBD8E817FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262DBFDC-115F-4452-9A80-75A422EFE86E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BCFEDF59-FA17-40DF-9E71-4D244AE6C829}"/>
   </bookViews>
@@ -415,7 +415,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +472,7 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement interaction with Aras Innovator server.
</commit_message>
<xml_diff>
--- a/Features To Implement.xlsx
+++ b/Features To Implement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\InnovatorDataModelEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981594FA-FFDD-4AA0-B447-00052C7245B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CB5330-E4C4-4F49-B5CE-1E0F41D66987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCFEDF59-FA17-40DF-9E71-4D244AE6C829}"/>
   </bookViews>
@@ -72,7 +72,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,12 +82,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -104,10 +98,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +418,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,7 +439,7 @@
         <f>B2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement interaction with AML.
</commit_message>
<xml_diff>
--- a/Features To Implement.xlsx
+++ b/Features To Implement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\InnovatorDataModelEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE59FAE-2B7D-4A78-B862-F70B32845A49}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981594FA-FFDD-4AA0-B447-00052C7245B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{BCFEDF59-FA17-40DF-9E71-4D244AE6C829}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCFEDF59-FA17-40DF-9E71-4D244AE6C829}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -69,7 +72,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +82,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -95,9 +104,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +425,7 @@
   <dimension ref="B2:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +437,7 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -436,7 +446,7 @@
         <f>B2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add custom property editors to TODO.
</commit_message>
<xml_diff>
--- a/Features To Implement.xlsx
+++ b/Features To Implement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\InnovatorDataModelEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CB5330-E4C4-4F49-B5CE-1E0F41D66987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585FC276-9366-4721-B61E-25262EF34287}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCFEDF59-FA17-40DF-9E71-4D244AE6C829}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Import/Export from/to AML</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Editing of ItemTypes has to be cancelable</t>
+  </si>
+  <si>
+    <t>Different editors for different property types</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214ADE4D-5369-492C-877A-701D588DFE45}">
-  <dimension ref="B2:C10"/>
+  <dimension ref="B2:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,7 +448,7 @@
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4">
-        <f t="shared" ref="B4:B10" si="0">B3+1</f>
+        <f t="shared" ref="B4:B11" si="0">B3+1</f>
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -501,6 +504,15 @@
       <c r="B10">
         <f t="shared" si="0"/>
         <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>